<commit_message>
fixed the animal scraping script
</commit_message>
<xml_diff>
--- a/Animals_Data.xlsx
+++ b/Animals_Data.xlsx
@@ -413,14 +413,312 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Fact</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Habitat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Lifespan</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Diet</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Lion</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>A lion's roar can be heard from 8 kilometers away.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Grasslands, savannas</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>10-14 years</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Carnivore</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Octopus</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>An octopus has three hearts.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Oceans, coral reefs</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1-2 years</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Carnivore</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Elephant</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Elephants can recognize themselves in a mirror.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Forests, savannas</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>60-70 years</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Herbivore</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Penguin</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Penguins can stay underwater for up to 27 minutes.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Antarctic coasts</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>15-20 years</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Carnivore</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Giraffe</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Giraffes have the same number of neck bones as humans.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>African savannas</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>25 years</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Herbivore</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kangaroo</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Kangaroos can leap up to 3 meters high.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Australian bushland</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>20 years</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Herbivore</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sloth</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Sloths can hold their breath for up to 40 minutes.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Central and South American rainforests</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>20-30 years</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Herbivore</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Cheetah</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Cheetahs are the fastest land animals, reaching 112 km/h.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>African savannas</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>10-12 years</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Carnivore</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Polar Bear</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Polar bears have black skin under their white fur.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Arctic regions</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>25-30 years</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Carnivore</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Chimpanzee</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Chimpanzees can use tools and solve problems.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>African forests</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>40-50 years</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Omnivore</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>